<commit_message>
Update Excel and Code
</commit_message>
<xml_diff>
--- a/Actual vs Plan.xlsx
+++ b/Actual vs Plan.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="53">
   <si>
     <t>date</t>
   </si>
@@ -1249,6 +1249,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1339,7 +1340,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000025-06C4-4EBD-9DB5-5F6028942F55}"/>
                 </c:ext>
@@ -1361,7 +1364,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000006-3293-492F-8385-7317FCBDA947}"/>
                 </c:ext>
@@ -1662,6 +1667,7 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
+              <c:layout/>
               <c:dLblPos val="t"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -1670,7 +1676,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000007-3293-492F-8385-7317FCBDA947}"/>
                 </c:ext>
@@ -1678,6 +1686,7 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="30"/>
+              <c:layout/>
               <c:dLblPos val="t"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -1686,7 +1695,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000000-3293-492F-8385-7317FCBDA947}"/>
                 </c:ext>
@@ -2104,6 +2115,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3825,6 +3837,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3889,6 +3902,7 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
+              <c:layout/>
               <c:dLblPos val="t"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -3897,7 +3911,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000016-48A3-4227-866C-E3F61A29B8C1}"/>
                 </c:ext>
@@ -3905,6 +3921,7 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="30"/>
+              <c:layout/>
               <c:dLblPos val="t"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -3913,7 +3930,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000012-48A3-4227-866C-E3F61A29B8C1}"/>
                 </c:ext>
@@ -4213,6 +4232,7 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
+              <c:layout/>
               <c:dLblPos val="t"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -4221,7 +4241,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000015-48A3-4227-866C-E3F61A29B8C1}"/>
                 </c:ext>
@@ -4229,6 +4251,7 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="30"/>
+              <c:layout/>
               <c:dLblPos val="t"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -4237,7 +4260,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000013-48A3-4227-866C-E3F61A29B8C1}"/>
                 </c:ext>
@@ -4535,6 +4560,7 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
+              <c:layout/>
               <c:dLblPos val="t"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -4543,7 +4569,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000003-48A3-4227-866C-E3F61A29B8C1}"/>
                 </c:ext>
@@ -4551,6 +4579,7 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="30"/>
+              <c:layout/>
               <c:dLblPos val="t"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -4559,7 +4588,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000002-48A3-4227-866C-E3F61A29B8C1}"/>
                 </c:ext>
@@ -4860,6 +4891,7 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
+              <c:layout/>
               <c:dLblPos val="t"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -4868,7 +4900,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000014-48A3-4227-866C-E3F61A29B8C1}"/>
                 </c:ext>
@@ -4876,6 +4910,7 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="30"/>
+              <c:layout/>
               <c:dLblPos val="t"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -4884,7 +4919,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000004-48A3-4227-866C-E3F61A29B8C1}"/>
                 </c:ext>
@@ -5301,6 +5338,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6337,6 +6375,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6401,6 +6440,7 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
+              <c:layout/>
               <c:dLblPos val="t"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -6409,7 +6449,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000004-DDA2-42C6-9491-EA0926A527DF}"/>
                 </c:ext>
@@ -6417,6 +6459,7 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="30"/>
+              <c:layout/>
               <c:dLblPos val="t"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -6425,7 +6468,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000004-8A28-4297-AE44-C665D87E7819}"/>
                 </c:ext>
@@ -6725,6 +6770,7 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="30"/>
+              <c:layout/>
               <c:dLblPos val="t"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -6733,7 +6779,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000005-8A28-4297-AE44-C665D87E7819}"/>
                 </c:ext>
@@ -7151,6 +7199,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -11933,7 +11982,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AH51" sqref="AH51"/>
+      <selection pane="bottomRight" activeCell="I48" sqref="I48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -16598,86 +16647,66 @@
         <v>46060</v>
       </c>
       <c r="D39" s="6">
-        <f>_xll.PIArcVal(Sheet1!$A$1,Sheet1!C39,0,"","auto")</f>
         <v>202.67999267578125</v>
       </c>
       <c r="E39" s="6">
-        <f>_xll.PIArcVal(Sheet1!$A$2,Sheet1!C39,0,"","auto")</f>
         <v>586.760009765625</v>
       </c>
       <c r="F39" s="7">
-        <f>_xll.PIArcVal(Sheet1!$A$3,Sheet1!C39,0,"","auto")</f>
         <v>419141</v>
       </c>
       <c r="G39" s="7">
-        <f>_xll.PIArcVal(Sheet1!$A$4,Sheet1!C39,0,"","auto")</f>
         <v>181582</v>
       </c>
       <c r="H39" s="6">
-        <f>_xll.PIArcVal(Sheet1!$A$5,Sheet1!C39,0,"","auto")</f>
         <v>46.290000915527344</v>
       </c>
       <c r="I39" s="6">
-        <f>_xll.PIArcVal(Sheet1!$A$6,Sheet1!C39,0,"","auto")</f>
         <v>53.180000305175781</v>
       </c>
       <c r="J39" s="6">
-        <f>_xll.PIArcVal(Sheet1!$A$7,Sheet1!C39,0,"","auto")</f>
         <v>56412</v>
       </c>
       <c r="K39" s="6">
-        <f>_xll.PIArcVal(Sheet1!$A$8,Sheet1!C39,0,"","auto")</f>
         <v>187621</v>
       </c>
       <c r="L39" s="6">
-        <f>_xll.PIArcVal(Sheet1!$A$9,Sheet1!C39,0,"","auto")</f>
         <v>1571.800048828125</v>
       </c>
       <c r="M39" s="6">
-        <f>_xll.PIArcVal(Sheet1!$A$10,Sheet1!C39,0,"","auto")</f>
         <v>1153.5400390625</v>
       </c>
       <c r="N39" s="8">
-        <f t="shared" ref="N39" si="11">(J39+F39-F38)/(D39*H39/100)/1000</f>
         <v>0.57431967992542365</v>
       </c>
       <c r="O39" s="8">
-        <f t="shared" ref="O39" si="12">(K39+G39-G38)/(E39*I39/100)/1000</f>
         <v>0.57431287232367023</v>
       </c>
       <c r="P39" s="8">
-        <f t="shared" ref="P39" si="13">((J39+K39)+F39+G39-F38-G38)/(D39*H39/100+E39*I39/100)/1000</f>
         <v>0.57431444600374548</v>
       </c>
       <c r="Q39" s="8">
-        <f t="shared" ref="Q39" si="14">P39*H39*10</f>
         <v>265.85016231313955</v>
       </c>
       <c r="R39" s="8">
-        <f t="shared" ref="R39" si="15">P39*I39*10</f>
         <v>305.42042413746049</v>
       </c>
       <c r="S39" s="4">
-        <f t="shared" ref="S39" si="16">((J39+K39)+F39+G39-F38-G38)/(D39+E39)</f>
         <v>295.26119689798776</v>
       </c>
       <c r="T39" s="5">
-        <f t="shared" ref="T39" si="17">IF(AL39&lt;3000,0,AL39)</f>
         <v>249405</v>
       </c>
       <c r="U39" s="5">
-        <f t="shared" ref="U39" si="18">IF(AM39&lt;3000,0,AM39)</f>
         <v>0</v>
       </c>
       <c r="V39" s="5">
-        <f t="shared" ref="V39" si="19">IF(AN39&lt;3000,0,AN39)</f>
         <v>0</v>
       </c>
       <c r="W39" s="5" t="s">
         <v>51</v>
       </c>
       <c r="X39" s="7">
-        <f t="shared" ref="X39" si="20">J39+K39</f>
         <v>244033</v>
       </c>
       <c r="Y39" s="4">
@@ -16717,19 +16746,15 @@
         <v>0</v>
       </c>
       <c r="AK39" s="4">
-        <f t="shared" ref="AK39" si="21">SUM(AH39:AJ39)</f>
         <v>250000</v>
       </c>
       <c r="AL39" s="5">
-        <f>_xll.PIArcVal(Sheet1!$A$11,Sheet1!C39,0,"","auto")</f>
         <v>249405</v>
       </c>
       <c r="AM39" s="5">
-        <f>_xll.PIArcVal(Sheet1!$A$12,Sheet1!C39,0,"","auto")</f>
         <v>530</v>
       </c>
       <c r="AN39" s="5">
-        <f>_xll.PIArcVal(Sheet1!$A$13,Sheet1!C39,0,"","auto")</f>
         <v>-13</v>
       </c>
     </row>
@@ -16740,43 +16765,117 @@
       <c r="C40" s="13">
         <v>46061</v>
       </c>
-      <c r="D40" s="4"/>
-      <c r="E40" s="4"/>
-      <c r="F40" s="4"/>
-      <c r="G40" s="4"/>
-      <c r="H40" s="4"/>
-      <c r="I40" s="4"/>
-      <c r="J40" s="4"/>
-      <c r="K40" s="4"/>
-      <c r="L40" s="4"/>
-      <c r="M40" s="4"/>
-      <c r="N40" s="4"/>
-      <c r="O40" s="4"/>
-      <c r="P40" s="4"/>
-      <c r="Q40" s="4"/>
-      <c r="R40" s="4"/>
-      <c r="S40" s="4"/>
-      <c r="T40" s="4"/>
-      <c r="U40" s="4"/>
-      <c r="V40" s="4"/>
-      <c r="W40" s="4"/>
-      <c r="X40" s="4"/>
-      <c r="Y40" s="4"/>
-      <c r="Z40" s="4"/>
-      <c r="AA40" s="4"/>
-      <c r="AB40" s="4"/>
-      <c r="AC40" s="4"/>
-      <c r="AD40" s="4"/>
-      <c r="AE40" s="4"/>
-      <c r="AF40" s="4"/>
-      <c r="AG40" s="4"/>
-      <c r="AH40" s="4"/>
-      <c r="AI40" s="4"/>
-      <c r="AJ40" s="4"/>
-      <c r="AK40" s="4"/>
-      <c r="AL40" s="4"/>
-      <c r="AM40" s="4"/>
-      <c r="AN40" s="4"/>
+      <c r="D40" s="6">
+        <v>511.80999755859375</v>
+      </c>
+      <c r="E40" s="6">
+        <v>365.79998779296875</v>
+      </c>
+      <c r="F40" s="7">
+        <v>422878</v>
+      </c>
+      <c r="G40" s="7">
+        <v>184666</v>
+      </c>
+      <c r="H40" s="6">
+        <v>45.580001831054688</v>
+      </c>
+      <c r="I40" s="6">
+        <v>52.610000610351563</v>
+      </c>
+      <c r="J40" s="6">
+        <v>136530</v>
+      </c>
+      <c r="K40" s="6">
+        <v>112631</v>
+      </c>
+      <c r="L40" s="6">
+        <v>1616.0999755859375</v>
+      </c>
+      <c r="M40" s="6">
+        <v>1365.0899658203125</v>
+      </c>
+      <c r="N40" s="8">
+        <v>0.60127397297184004</v>
+      </c>
+      <c r="O40" s="8">
+        <v>0.60128125682479905</v>
+      </c>
+      <c r="P40" s="8">
+        <v>0.60127726556839112</v>
+      </c>
+      <c r="Q40" s="8">
+        <v>274.06218865578819</v>
+      </c>
+      <c r="R40" s="8">
+        <v>316.33197308543578</v>
+      </c>
+      <c r="S40" s="4">
+        <v>291.68081980910455</v>
+      </c>
+      <c r="T40" s="5">
+        <v>243968</v>
+      </c>
+      <c r="U40" s="5">
+        <v>0</v>
+      </c>
+      <c r="V40" s="5">
+        <v>0</v>
+      </c>
+      <c r="W40" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="X40" s="7">
+        <v>249161</v>
+      </c>
+      <c r="Y40" s="4">
+        <v>0.61699999999999999</v>
+      </c>
+      <c r="Z40" s="9">
+        <v>0.624</v>
+      </c>
+      <c r="AA40" s="9">
+        <v>0.62</v>
+      </c>
+      <c r="AB40" s="9">
+        <v>264.32</v>
+      </c>
+      <c r="AC40" s="9">
+        <v>323.33999999999997</v>
+      </c>
+      <c r="AD40" s="4">
+        <v>44.27</v>
+      </c>
+      <c r="AE40" s="4">
+        <v>52.51</v>
+      </c>
+      <c r="AF40" s="9">
+        <v>1369.99</v>
+      </c>
+      <c r="AG40" s="9">
+        <v>1287.671</v>
+      </c>
+      <c r="AH40" s="4">
+        <v>250000</v>
+      </c>
+      <c r="AI40" s="9">
+        <v>0</v>
+      </c>
+      <c r="AJ40" s="9">
+        <v>0</v>
+      </c>
+      <c r="AK40" s="4">
+        <v>250000</v>
+      </c>
+      <c r="AL40" s="5">
+        <v>243968</v>
+      </c>
+      <c r="AM40" s="5">
+        <v>92</v>
+      </c>
+      <c r="AN40" s="5">
+        <v>-27</v>
+      </c>
     </row>
     <row r="41" spans="2:40">
       <c r="B41" s="20">
@@ -16785,43 +16884,141 @@
       <c r="C41" s="13">
         <v>46062</v>
       </c>
-      <c r="D41" s="4"/>
-      <c r="E41" s="4"/>
-      <c r="F41" s="4"/>
-      <c r="G41" s="4"/>
-      <c r="H41" s="4"/>
-      <c r="I41" s="4"/>
-      <c r="J41" s="4"/>
-      <c r="K41" s="4"/>
-      <c r="L41" s="4"/>
-      <c r="M41" s="4"/>
-      <c r="N41" s="4"/>
-      <c r="O41" s="4"/>
-      <c r="P41" s="4"/>
-      <c r="Q41" s="4"/>
-      <c r="R41" s="4"/>
-      <c r="S41" s="4"/>
-      <c r="T41" s="4"/>
-      <c r="U41" s="4"/>
-      <c r="V41" s="4"/>
-      <c r="W41" s="4"/>
-      <c r="X41" s="4"/>
-      <c r="Y41" s="4"/>
-      <c r="Z41" s="4"/>
-      <c r="AA41" s="4"/>
-      <c r="AB41" s="4"/>
-      <c r="AC41" s="4"/>
-      <c r="AD41" s="4"/>
-      <c r="AE41" s="4"/>
-      <c r="AF41" s="4"/>
-      <c r="AG41" s="4"/>
-      <c r="AH41" s="4"/>
-      <c r="AI41" s="4"/>
-      <c r="AJ41" s="4"/>
-      <c r="AK41" s="4"/>
-      <c r="AL41" s="4"/>
-      <c r="AM41" s="4"/>
-      <c r="AN41" s="4"/>
+      <c r="D41" s="6">
+        <f>_xll.PIArcVal(Sheet1!$A$1,Sheet1!C41,0,"","auto")</f>
+        <v>325.8699951171875</v>
+      </c>
+      <c r="E41" s="6">
+        <f>_xll.PIArcVal(Sheet1!$A$2,Sheet1!C41,0,"","auto")</f>
+        <v>532.15997314453125</v>
+      </c>
+      <c r="F41" s="7">
+        <f>_xll.PIArcVal(Sheet1!$A$3,Sheet1!C41,0,"","auto")</f>
+        <v>416906</v>
+      </c>
+      <c r="G41" s="7">
+        <f>_xll.PIArcVal(Sheet1!$A$4,Sheet1!C41,0,"","auto")</f>
+        <v>172831</v>
+      </c>
+      <c r="H41" s="6">
+        <f>_xll.PIArcVal(Sheet1!$A$5,Sheet1!C41,0,"","auto")</f>
+        <v>43.009998321533203</v>
+      </c>
+      <c r="I41" s="6">
+        <f>_xll.PIArcVal(Sheet1!$A$6,Sheet1!C41,0,"","auto")</f>
+        <v>52.189998626708984</v>
+      </c>
+      <c r="J41" s="6">
+        <f>_xll.PIArcVal(Sheet1!$A$7,Sheet1!C41,0,"","auto")</f>
+        <v>87671</v>
+      </c>
+      <c r="K41" s="6">
+        <f>_xll.PIArcVal(Sheet1!$A$8,Sheet1!C41,0,"","auto")</f>
+        <v>173729</v>
+      </c>
+      <c r="L41" s="6">
+        <f>_xll.PIArcVal(Sheet1!$A$9,Sheet1!C41,0,"","auto")</f>
+        <v>1141.699951171875</v>
+      </c>
+      <c r="M41" s="6">
+        <f>_xll.PIArcVal(Sheet1!$A$10,Sheet1!C41,0,"","auto")</f>
+        <v>1405.5400390625</v>
+      </c>
+      <c r="N41" s="8">
+        <f t="shared" ref="N41" si="11">(J41+F41-F40)/(D41*H41/100)/1000</f>
+        <v>0.58291192636765532</v>
+      </c>
+      <c r="O41" s="8">
+        <f t="shared" ref="O41" si="12">(K41+G41-G40)/(E41*I41/100)/1000</f>
+        <v>0.58290967337600053</v>
+      </c>
+      <c r="P41" s="8">
+        <f t="shared" ref="P41" si="13">((J41+K41)+F41+G41-F40-G40)/(D41*H41/100+E41*I41/100)/1000</f>
+        <v>0.58291042900810974</v>
+      </c>
+      <c r="Q41" s="8">
+        <f t="shared" ref="Q41" si="14">P41*H41*10</f>
+        <v>250.70976573242999</v>
+      </c>
+      <c r="R41" s="8">
+        <f t="shared" ref="R41" si="15">P41*I41*10</f>
+        <v>304.22094489427593</v>
+      </c>
+      <c r="S41" s="4">
+        <f t="shared" ref="S41" si="16">((J41+K41)+F41+G41-F40-G40)/(D41+E41)</f>
+        <v>283.89800940577237</v>
+      </c>
+      <c r="T41" s="5">
+        <f t="shared" ref="T41" si="17">IF(AL41&lt;3000,0,AL41)</f>
+        <v>261643</v>
+      </c>
+      <c r="U41" s="5">
+        <f t="shared" ref="U41" si="18">IF(AM41&lt;3000,0,AM41)</f>
+        <v>0</v>
+      </c>
+      <c r="V41" s="5">
+        <f t="shared" ref="V41" si="19">IF(AN41&lt;3000,0,AN41)</f>
+        <v>0</v>
+      </c>
+      <c r="W41" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="X41" s="7">
+        <f t="shared" ref="X41" si="20">J41+K41</f>
+        <v>261400</v>
+      </c>
+      <c r="Y41" s="4">
+        <v>0.61699999999999999</v>
+      </c>
+      <c r="Z41" s="9">
+        <v>0.624</v>
+      </c>
+      <c r="AA41" s="9">
+        <v>0.62</v>
+      </c>
+      <c r="AB41" s="9">
+        <v>264.32</v>
+      </c>
+      <c r="AC41" s="9">
+        <v>323.33999999999997</v>
+      </c>
+      <c r="AD41" s="4">
+        <v>44.27</v>
+      </c>
+      <c r="AE41" s="4">
+        <v>52.51</v>
+      </c>
+      <c r="AF41" s="9">
+        <v>1369.99</v>
+      </c>
+      <c r="AG41" s="9">
+        <v>1287.671</v>
+      </c>
+      <c r="AH41" s="4">
+        <v>250000</v>
+      </c>
+      <c r="AI41" s="9">
+        <v>0</v>
+      </c>
+      <c r="AJ41" s="9">
+        <v>0</v>
+      </c>
+      <c r="AK41" s="4">
+        <f t="shared" ref="AK41" si="21">SUM(AH41:AJ41)</f>
+        <v>250000</v>
+      </c>
+      <c r="AL41" s="5">
+        <f>_xll.PIArcVal(Sheet1!$A$11,Sheet1!C41,0,"","auto")</f>
+        <v>261643</v>
+      </c>
+      <c r="AM41" s="5">
+        <f>_xll.PIArcVal(Sheet1!$A$12,Sheet1!C41,0,"","auto")</f>
+        <v>-274</v>
+      </c>
+      <c r="AN41" s="5">
+        <f>_xll.PIArcVal(Sheet1!$A$13,Sheet1!C41,0,"","auto")</f>
+        <v>31</v>
+      </c>
     </row>
     <row r="42" spans="2:40">
       <c r="B42" s="20">

</xml_diff>